<commit_message>
Some changes in excel support and AreEqual bug fix
</commit_message>
<xml_diff>
--- a/storage/excel/fixtures/test.xlsx
+++ b/storage/excel/fixtures/test.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5C69489-0617-47A0-804B-D2476CE3EA37}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B62E062-31CA-4EE5-9939-45E3A777D115}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10740" yWindow="2835" windowWidth="13260" windowHeight="12765" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14616" yWindow="1944" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="TestingSheet" sheetId="3" r:id="rId2"/>
-    <sheet name="CustomSheet" sheetId="2" r:id="rId3"/>
+    <sheet name="CustomSheet" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Jan</t>
   </si>
@@ -63,10 +62,16 @@
     <t>Miami</t>
   </si>
   <si>
-    <t>Id</t>
-  </si>
-  <si>
     <t>points</t>
+  </si>
+  <si>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Ally</t>
   </si>
 </sst>
 </file>
@@ -106,7 +111,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -387,12 +392,12 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="A1:C5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -403,7 +408,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -414,7 +419,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -425,7 +430,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -442,134 +447,109 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBCAEE51-99A6-4619-B9F2-588434155E0E}">
-  <dimension ref="C4:E7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09FD147E-6F7D-4AE6-9998-136D76D2D958}">
+  <dimension ref="A2:F12"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AA1" sqref="AA1"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1700000</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>2000</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="B9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>13</v>
+      </c>
+      <c r="C10">
         <v>1</v>
       </c>
-      <c r="E5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7">
-        <v>21</v>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F121D870-42DD-439E-B266-2CE1AE712343}">
-  <dimension ref="B2:F6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>1700000</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4">
-        <v>2000</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-      <c r="F4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="E5">
-        <v>3</v>
-      </c>
-      <c r="F5">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6">
-        <v>-5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Excel date support + time parse modification + tests
</commit_message>
<xml_diff>
--- a/storage/excel/fixtures/test.xlsx
+++ b/storage/excel/fixtures/test.xlsx
@@ -3,25 +3,32 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B62E062-31CA-4EE5-9939-45E3A777D115}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310EFE82-9D84-42C7-B16D-6EECEE5E8531}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14616" yWindow="1944" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="1944" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="CustomSheet" sheetId="5" r:id="rId2"/>
+    <sheet name="DateSheet" sheetId="6" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>Jan</t>
   </si>
@@ -72,12 +79,20 @@
   </si>
   <si>
     <t>Ally</t>
+  </si>
+  <si>
+    <t>date</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="166" formatCode="dd\-mm\-yy\ h:mm;@"/>
+    <numFmt numFmtId="171" formatCode="[$-409]dd\-mm\-yy\ h:mm\ AM/PM;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -107,8 +122,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,7 +469,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09FD147E-6F7D-4AE6-9998-136D76D2D958}">
   <dimension ref="A2:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -552,4 +571,82 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3491787D-376F-417A-B5F9-4BDBE24B2915}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.21875" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>42808.541666666664</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>42809.541666608799</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>43604.583333333336</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="D4" s="4">
+        <v>42808.541666666664</v>
+      </c>
+      <c r="E4">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D5" s="4">
+        <v>42809.541666608799</v>
+      </c>
+      <c r="E5">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D6" s="4">
+        <v>43604.583333333336</v>
+      </c>
+      <c r="E6">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>